<commit_message>
Extended features for RC2025 rule revisions
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\Downloads\3d Printing\RoboCup Ramp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3A3B11D-385B-42B0-AE85-CCD1BBA99427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{E3A3B11D-385B-42B0-AE85-CCD1BBA99427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB305F8-436A-47B8-927D-E1CAF24EF35D}"/>
   <bookViews>
     <workbookView xWindow="12570" yWindow="2220" windowWidth="19425" windowHeight="15405" xr2:uid="{A429339D-88C0-48D5-BAF1-117506D41BB5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Component</t>
   </si>
@@ -59,7 +59,7 @@
     <t>ISO 4762 / DIN 912</t>
   </si>
   <si>
-    <t>Button head screws won't work due to its head size</t>
+    <t>Button head screws won't work due to its head size, Hex is preferred for its resilience against stripping</t>
   </si>
   <si>
     <t>AliExpress</t>
@@ -68,16 +68,34 @@
     <t>M3x8 BHCS</t>
   </si>
   <si>
-    <t>Hex is preferred for its resilience against stripping</t>
-  </si>
-  <si>
     <t>M3x10 BHCS</t>
   </si>
   <si>
     <t>M3x4x5 Brass Heatset Insert</t>
   </si>
   <si>
-    <t>M3 insert, 4mm OD, 5mm Length (shorter length could still work)</t>
+    <t>18 is needed if extension is used, M3 insert, 4mm OD, 5mm Length (shorter length could still work)</t>
+  </si>
+  <si>
+    <t>Extensions extra optional</t>
+  </si>
+  <si>
+    <t>Add these numbers up for each extension that you are using</t>
+  </si>
+  <si>
+    <t>Base extension screws</t>
+  </si>
+  <si>
+    <t>Ramp extension screws</t>
+  </si>
+  <si>
+    <t>4 is needed for a base extension</t>
+  </si>
+  <si>
+    <t>4 or 6</t>
+  </si>
+  <si>
+    <t>4 is needed for a ramp extension if you are using a base extension, if you aren't then you need 6</t>
   </si>
   <si>
     <t>Other tools needed</t>
@@ -93,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +132,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,10 +161,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -476,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935B6377-BEF6-4E45-AB69-9B985D9BA588}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -487,7 +521,7 @@
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="58.5703125" customWidth="1"/>
+    <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,11 +566,8 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -544,7 +575,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -558,13 +589,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -572,20 +603,81 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{9CEEF204-5297-4DCF-9F11-6AC113139223}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{9120CA06-C1BA-4562-91FF-F9A47E376260}"/>
@@ -593,6 +685,9 @@
     <hyperlink ref="E2" r:id="rId4" xr:uid="{0BF26C9D-E2B8-4CDD-9214-7EE0C61FD167}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;KFFFF00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -606,8 +701,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090EEB4B15F66A4438E506D2218BC0A7D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6b3154bdc57b1c6a307ce3d00ac3556f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcb42a41-c19f-4816-b129-11987572b47a" xmlns:ns3="56e4a4f7-f59c-4e24-9e36-e380214a8d94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ee5187c4d9cd08aa38b7ccfdf4e3773" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090EEB4B15F66A4438E506D2218BC0A7D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7552855a4c84ead4d675dc1e5af80b25">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcb42a41-c19f-4816-b129-11987572b47a" xmlns:ns3="56e4a4f7-f59c-4e24-9e36-e380214a8d94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1282705512627f5a642b39c779e8d4a8" ns2:_="" ns3:_="">
     <xsd:import namespace="bcb42a41-c19f-4816-b129-11987572b47a"/>
     <xsd:import namespace="56e4a4f7-f59c-4e24-9e36-e380214a8d94"/>
     <xsd:element name="properties">
@@ -630,6 +725,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -695,6 +791,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="23" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -856,9 +957,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1BFE74-CF44-4465-8E9F-A4403D6C8EAF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F110C687-2037-4787-AB33-F63EF168C306}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4C8F47-C874-4DFD-80E8-8230F61C4387}"/>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{8c3d088b-6243-4963-a2e2-8b321ab7f8fc}" enabled="1" method="Standard" siteId="{d1323671-cdbe-4417-b4d4-bdb24b51316b}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>